<commit_message>
Report with all diagrams
</commit_message>
<xml_diff>
--- a/lab1/lab1Report.xlsx
+++ b/lab1/lab1Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\university\combinate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\2Attempt\university\combinate\lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -55,8 +52,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.000_ ;\-0.000\ "/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000_ ;\-0.000\ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -172,11 +169,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -272,7 +269,7 @@
             <c:numRef>
               <c:f>Лист1!$C$6:$H$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>3.1E-2</c:v>
@@ -305,11 +302,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="252430120"/>
-        <c:axId val="252432472"/>
+        <c:axId val="301977560"/>
+        <c:axId val="301974032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="252430120"/>
+        <c:axId val="301977560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -338,12 +335,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="252432472"/>
+        <c:crossAx val="301974032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="252432472"/>
+        <c:axId val="301974032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -374,11 +371,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="252430120"/>
+        <c:crossAx val="301977560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -468,7 +465,7 @@
             <c:numRef>
               <c:f>Лист1!$C$10:$H$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.6E-2</c:v>
@@ -501,11 +498,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="252432864"/>
-        <c:axId val="252433256"/>
+        <c:axId val="301977952"/>
+        <c:axId val="301974424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="252432864"/>
+        <c:axId val="301977952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -539,12 +536,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="252433256"/>
+        <c:crossAx val="301974424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="252433256"/>
+        <c:axId val="301974424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -575,11 +572,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="252432864"/>
+        <c:crossAx val="301977952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -641,7 +638,7 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:xVal>
             <c:numRef>
@@ -674,7 +671,66 @@
             <c:numRef>
               <c:f>Лист1!$C$14:$H$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.265999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>74.126000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$C$13:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$C$14:$H$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>4.7E-2</c:v>
@@ -707,11 +763,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="251357848"/>
-        <c:axId val="251361376"/>
+        <c:axId val="331343392"/>
+        <c:axId val="300833616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="251357848"/>
+        <c:axId val="331343392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -740,12 +796,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="251361376"/>
+        <c:crossAx val="300833616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="251361376"/>
+        <c:axId val="300833616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -771,11 +827,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="251357848"/>
+        <c:crossAx val="331343392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -865,7 +921,7 @@
             <c:numRef>
               <c:f>Лист1!$C$18:$H$18</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.4999999999999999E-2</c:v>
@@ -882,7 +938,7 @@
                 <c:pt idx="4">
                   <c:v>4.7649999999999997</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="5" formatCode="0.000_ ;\-0.000\ ">
                   <c:v>19.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -898,11 +954,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="251360200"/>
-        <c:axId val="251358240"/>
+        <c:axId val="301975208"/>
+        <c:axId val="301975600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="251360200"/>
+        <c:axId val="301975208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,12 +992,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="251358240"/>
+        <c:crossAx val="301975600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="251358240"/>
+        <c:axId val="301975600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -972,15 +1028,404 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="251360200"/>
+        <c:crossAx val="301975208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Сводная</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> таблица</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>InsertionSort</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$C$5:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$C$6:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.1E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.8E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.59399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.781000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45.078000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>InsertionBinarySort</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$C$9:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$C$10:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.6E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.20300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54700000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8439999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.39</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>BubbleSort</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$C$13:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$C$14:$H$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.265999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>74.126000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>SelectionSort</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$C$17:$H$17</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$C$18:$H$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.8E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.313</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.234</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.7649999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="334170184"/>
+        <c:axId val="334169400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="334170184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Количество элементов в массиве</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="334169400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="334169400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Время работы алгоритма, с</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="334170184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1061,16 +1506,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>72389</xdr:rowOff>
+      <xdr:rowOff>102869</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1905</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1123,20 +1568,39 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Диаграмма 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Лист1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1404,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>